<commit_message>
Added TS922, updated BC324
</commit_message>
<xml_diff>
--- a/Elektor-Labs-Preferred-Parts-(ELPP)-SMT-v1.0.xlsx
+++ b/Elektor-Labs-Preferred-Parts-(ELPP)-SMT-v1.0.xlsx
@@ -10,14 +10,14 @@
     <sheet name="THT" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">THT!$A$1:$I$224</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">THT!$A$1:$I$225</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1183" uniqueCount="669">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1189" uniqueCount="672">
   <si>
     <t>Description</t>
   </si>
@@ -2124,6 +2124,15 @@
   </si>
   <si>
     <t>538-2313</t>
+  </si>
+  <si>
+    <t>TS922, dual opamp, R2R IO, 4 MHz</t>
+  </si>
+  <si>
+    <t>TS922IDT</t>
+  </si>
+  <si>
+    <t>714-1142</t>
   </si>
 </sst>
 </file>
@@ -2683,10 +2692,10 @@
   <sheetPr codeName="Feuil1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M302"/>
+  <dimension ref="A1:M303"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="I167" sqref="I167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6808,19 +6817,19 @@
         <v>69</v>
       </c>
       <c r="K165" s="6" t="str">
-        <f t="shared" ref="K165:K169" si="7">CONCATENATE(CONCATENATE($E165,IF(ISBLANK($E165),""," = "),$A165),IF(ISBLANK($J165),"",", "),$J165)</f>
+        <f t="shared" ref="K165:K170" si="7">CONCATENATE(CONCATENATE($E165,IF(ISBLANK($E165),""," = "),$A165),IF(ISBLANK($J165),"",", "),$J165)</f>
         <v>IC = LM358, dual opamp</v>
       </c>
     </row>
     <row r="166" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A166" s="18" t="s">
-        <v>617</v>
+        <v>669</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>618</v>
+        <v>670</v>
       </c>
       <c r="D166" s="1" t="s">
         <v>383</v>
@@ -6829,148 +6838,145 @@
         <v>44</v>
       </c>
       <c r="G166" s="2">
+        <v>1642724</v>
+      </c>
+      <c r="I166" s="19" t="s">
+        <v>671</v>
+      </c>
+      <c r="K166" s="6"/>
+    </row>
+    <row r="167" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="A167" s="18" t="s">
+        <v>617</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C167" s="1" t="s">
+        <v>618</v>
+      </c>
+      <c r="D167" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="E167" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G167" s="2">
         <v>9490043</v>
       </c>
-      <c r="I166" s="19" t="s">
+      <c r="I167" s="19" t="s">
         <v>619</v>
       </c>
-      <c r="K166" s="6" t="str">
+      <c r="K167" s="6" t="str">
         <f t="shared" si="7"/>
         <v>IC = LM6132AIM, dual opamp, R2R, 10 MHz</v>
       </c>
     </row>
-    <row r="167" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="A167" s="18" t="s">
+    <row r="168" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="A168" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="B167" s="1" t="s">
+      <c r="B168" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C167" s="1" t="s">
+      <c r="C168" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="D167" s="1" t="s">
+      <c r="D168" s="1" t="s">
         <v>612</v>
       </c>
-      <c r="E167" s="1" t="s">
+      <c r="E168" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G167" s="2">
+      <c r="G168" s="2">
         <v>8389233</v>
       </c>
-      <c r="I167" s="19" t="s">
+      <c r="I168" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="K167" s="6" t="str">
+      <c r="K168" s="6" t="str">
         <f t="shared" si="7"/>
         <v>IC = LM324, quad opamp</v>
       </c>
     </row>
-    <row r="168" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="A168" s="18" t="s">
+    <row r="169" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="A169" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="B168" s="1" t="s">
+      <c r="B169" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C168" s="1" t="s">
+      <c r="C169" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="D168" s="1" t="s">
+      <c r="D169" s="1" t="s">
         <v>612</v>
       </c>
-      <c r="E168" s="1" t="s">
+      <c r="E169" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G168" s="2">
+      <c r="G169" s="2">
         <v>1750170</v>
       </c>
-      <c r="I168" s="19" t="s">
+      <c r="I169" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="K168" s="6" t="str">
+      <c r="K169" s="6" t="str">
         <f t="shared" si="7"/>
         <v>IC = TS924A, quad opamp, R2R IO, 4 MHz</v>
       </c>
     </row>
-    <row r="169" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="A169" s="18" t="s">
+    <row r="170" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="A170" s="18" t="s">
         <v>620</v>
       </c>
-      <c r="B169" s="1" t="s">
+      <c r="B170" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C169" s="1" t="s">
+      <c r="C170" s="1" t="s">
         <v>621</v>
       </c>
-      <c r="D169" s="1" t="s">
+      <c r="D170" s="1" t="s">
         <v>612</v>
       </c>
-      <c r="E169" s="1" t="s">
+      <c r="E170" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G169" s="2">
+      <c r="G170" s="2">
         <v>9490035</v>
       </c>
-      <c r="I169" s="19" t="s">
+      <c r="I170" s="19" t="s">
         <v>622</v>
       </c>
-      <c r="K169" s="6" t="str">
+      <c r="K170" s="6" t="str">
         <f t="shared" si="7"/>
         <v>IC = LM6134AIM, quad opamp, R2R, 10 MHz</v>
       </c>
     </row>
-    <row r="170" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="K170" s="6"/>
-    </row>
-    <row r="171" spans="1:11" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A171" s="14" t="s">
+    <row r="171" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="K171" s="6"/>
+    </row>
+    <row r="172" spans="1:11" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A172" s="14" t="s">
         <v>337</v>
       </c>
-      <c r="B171" s="14"/>
-      <c r="C171" s="14"/>
-      <c r="D171" s="14"/>
-      <c r="E171" s="14" t="s">
+      <c r="B172" s="14"/>
+      <c r="C172" s="14"/>
+      <c r="D172" s="14"/>
+      <c r="E172" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="K171" s="17"/>
-    </row>
-    <row r="172" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="A172" s="18" t="s">
-        <v>345</v>
-      </c>
-      <c r="B172" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C172" s="1" t="s">
-        <v>344</v>
-      </c>
-      <c r="D172" s="1" t="s">
-        <v>613</v>
-      </c>
-      <c r="E172" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G172" s="2">
-        <v>2328475</v>
-      </c>
-      <c r="I172" s="2" t="s">
-        <v>572</v>
-      </c>
-      <c r="K172" s="6" t="str">
-        <f t="shared" ref="K172:K203" si="8">CONCATENATE(CONCATENATE($E172,IF(ISBLANK($E172),""," = "),$A172),IF(ISBLANK($J172),"",", "),$J172)</f>
-        <v>P = 1 kΩ, trimmer, 4.5 mm, 250 mW</v>
-      </c>
+      <c r="K172" s="17"/>
     </row>
     <row r="173" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A173" s="18" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B173" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="D173" s="1" t="s">
         <v>613</v>
@@ -6978,697 +6984,697 @@
       <c r="E173" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F173" s="2">
+      <c r="G173" s="2">
+        <v>2328475</v>
+      </c>
+      <c r="I173" s="2" t="s">
+        <v>572</v>
+      </c>
+      <c r="K173" s="6" t="str">
+        <f t="shared" ref="K173:K204" si="8">CONCATENATE(CONCATENATE($E173,IF(ISBLANK($E173),""," = "),$A173),IF(ISBLANK($J173),"",", "),$J173)</f>
+        <v>P = 1 kΩ, trimmer, 4.5 mm, 250 mW</v>
+      </c>
+    </row>
+    <row r="174" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="A174" s="18" t="s">
+        <v>346</v>
+      </c>
+      <c r="B174" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C174" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="D174" s="1" t="s">
+        <v>613</v>
+      </c>
+      <c r="E174" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F174" s="2">
         <v>2328486</v>
       </c>
-      <c r="G173" s="2">
+      <c r="G174" s="2">
         <v>2328486</v>
       </c>
-      <c r="I173" s="2" t="s">
+      <c r="I174" s="2" t="s">
         <v>573</v>
       </c>
-      <c r="K173" s="6" t="str">
+      <c r="K174" s="6" t="str">
         <f t="shared" si="8"/>
         <v>P = 5 kΩ, trimmer, 4.5 mm, 250 mW</v>
       </c>
     </row>
-    <row r="174" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="A174" s="18" t="s">
+    <row r="175" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="A175" s="18" t="s">
         <v>347</v>
       </c>
-      <c r="B174" s="1" t="s">
+      <c r="B175" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C174" s="1" t="s">
+      <c r="C175" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="D174" s="1" t="s">
+      <c r="D175" s="1" t="s">
         <v>613</v>
       </c>
-      <c r="E174" s="1" t="s">
+      <c r="E175" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="G174" s="2">
+      <c r="G175" s="2">
         <v>2328476</v>
       </c>
-      <c r="I174" s="2" t="s">
+      <c r="I175" s="2" t="s">
         <v>574</v>
       </c>
-      <c r="K174" s="6" t="str">
+      <c r="K175" s="6" t="str">
         <f t="shared" si="8"/>
         <v>P = 10 kΩ, trimmer, 4.5 mm, 250 mW</v>
       </c>
     </row>
-    <row r="175" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="A175" s="18" t="s">
+    <row r="176" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="A176" s="18" t="s">
         <v>348</v>
       </c>
-      <c r="B175" s="1" t="s">
+      <c r="B176" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C175" s="1" t="s">
+      <c r="C176" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="D175" s="1" t="s">
+      <c r="D176" s="1" t="s">
         <v>613</v>
       </c>
-      <c r="E175" s="1" t="s">
+      <c r="E176" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="G175" s="2">
+      <c r="G176" s="2">
         <v>2328487</v>
       </c>
-      <c r="I175" s="2" t="s">
+      <c r="I176" s="2" t="s">
         <v>575</v>
       </c>
-      <c r="K175" s="6" t="str">
+      <c r="K176" s="6" t="str">
         <f t="shared" si="8"/>
         <v>P = 47 kΩ, trimmer, 4.5 mm, 250 mW</v>
       </c>
     </row>
-    <row r="176" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="A176" s="18" t="s">
+    <row r="177" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="A177" s="18" t="s">
         <v>349</v>
       </c>
-      <c r="B176" s="1" t="s">
+      <c r="B177" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C176" s="1" t="s">
+      <c r="C177" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="D176" s="1" t="s">
+      <c r="D177" s="1" t="s">
         <v>613</v>
       </c>
-      <c r="E176" s="1" t="s">
+      <c r="E177" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="G176" s="2">
+      <c r="G177" s="2">
         <v>2328477</v>
       </c>
-      <c r="I176" s="2" t="s">
+      <c r="I177" s="2" t="s">
         <v>576</v>
       </c>
-      <c r="K176" s="6" t="str">
+      <c r="K177" s="6" t="str">
         <f t="shared" si="8"/>
         <v>P = 100 kΩ, trimmer, 4.5 mm, 250 mW</v>
       </c>
     </row>
-    <row r="177" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="A177" s="18" t="s">
+    <row r="178" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="A178" s="18" t="s">
         <v>339</v>
       </c>
-      <c r="B177" s="1" t="s">
+      <c r="B178" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C177" s="1" t="s">
+      <c r="C178" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="D177" s="1" t="s">
+      <c r="D178" s="1" t="s">
         <v>613</v>
       </c>
-      <c r="E177" s="1" t="s">
+      <c r="E178" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="G177" s="2">
+      <c r="G178" s="2">
         <v>2328478</v>
       </c>
-      <c r="I177" s="2" t="s">
+      <c r="I178" s="2" t="s">
         <v>577</v>
       </c>
-      <c r="K177" s="6" t="str">
+      <c r="K178" s="6" t="str">
         <f t="shared" si="8"/>
         <v>P = 1 MΩ, trimmer, 4.5 mm, 250 mW</v>
       </c>
     </row>
-    <row r="178" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="A178" s="2"/>
-      <c r="K178" s="6" t="str">
+    <row r="179" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="A179" s="2"/>
+      <c r="K179" s="6" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
-    <row r="179" spans="1:11" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A179" s="14" t="s">
+    <row r="180" spans="1:11" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A180" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="B179" s="14"/>
-      <c r="C179" s="14"/>
-      <c r="D179" s="14"/>
-      <c r="E179" s="14"/>
-      <c r="K179" s="17" t="str">
+      <c r="B180" s="14"/>
+      <c r="C180" s="14"/>
+      <c r="D180" s="14"/>
+      <c r="E180" s="14"/>
+      <c r="K180" s="17" t="str">
         <f t="shared" si="8"/>
         <v>Thyristor</v>
       </c>
     </row>
-    <row r="180" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="A180" s="18" t="s">
+    <row r="181" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="A181" s="18" t="s">
         <v>351</v>
       </c>
-      <c r="B180" s="1" t="s">
+      <c r="B181" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C180" s="1" t="s">
+      <c r="C181" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="D180" s="1" t="s">
+      <c r="D181" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="E180" s="1" t="s">
+      <c r="E181" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G180" s="2">
+      <c r="G181" s="2">
         <v>1689300</v>
       </c>
-      <c r="I180" s="2" t="s">
+      <c r="I181" s="2" t="s">
         <v>578</v>
       </c>
-      <c r="K180" s="6" t="str">
+      <c r="K181" s="6" t="str">
         <f t="shared" si="8"/>
         <v>DI = DIAC, 32 V, 1 A</v>
       </c>
     </row>
-    <row r="181" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="A181" s="18" t="s">
+    <row r="182" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="A182" s="18" t="s">
         <v>352</v>
       </c>
-      <c r="B181" s="1" t="s">
+      <c r="B182" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C181" s="1" t="s">
+      <c r="C182" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="D181" s="1" t="s">
+      <c r="D182" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="E181" s="1" t="s">
+      <c r="E182" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G181" s="2">
+      <c r="G182" s="2">
         <v>2341673</v>
       </c>
-      <c r="I181" s="33" t="s">
+      <c r="I182" s="33" t="s">
         <v>580</v>
       </c>
-      <c r="K181" s="6" t="str">
+      <c r="K182" s="6" t="str">
         <f t="shared" si="8"/>
         <v>TH = TS820-600B, SCR, 600 V, 8 A (RMS), 0.2 mA</v>
       </c>
     </row>
-    <row r="182" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="A182" s="18" t="s">
+    <row r="183" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="A183" s="18" t="s">
         <v>357</v>
       </c>
-      <c r="B182" s="1" t="s">
+      <c r="B183" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C182" s="1" t="s">
+      <c r="C183" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="D182" s="1" t="s">
+      <c r="D183" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="E182" s="1" t="s">
+      <c r="E183" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="G182" s="2">
+      <c r="G183" s="2">
         <v>1757883</v>
       </c>
-      <c r="I182" s="2" t="s">
+      <c r="I183" s="2" t="s">
         <v>579</v>
       </c>
-      <c r="K182" s="6" t="str">
+      <c r="K183" s="6" t="str">
         <f t="shared" si="8"/>
         <v>TRI = BT137S-600D, TRIAC, 600 V, 8 A (RMS), 10 mA</v>
       </c>
     </row>
-    <row r="183" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="K183" s="6" t="str">
+    <row r="184" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="K184" s="6" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
-    <row r="184" spans="1:11" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A184" s="7" t="s">
+    <row r="185" spans="1:11" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A185" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B184" s="7"/>
-      <c r="C184" s="7"/>
-      <c r="D184" s="7"/>
-      <c r="E184" s="7" t="s">
+      <c r="B185" s="7"/>
+      <c r="C185" s="7"/>
+      <c r="D185" s="7"/>
+      <c r="E185" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="K184" s="9" t="str">
+      <c r="K185" s="9" t="str">
         <f t="shared" si="8"/>
         <v>T = Transistor BJT NPN</v>
       </c>
     </row>
-    <row r="185" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="A185" s="18" t="s">
+    <row r="186" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="A186" s="18" t="s">
         <v>366</v>
       </c>
-      <c r="B185" s="1" t="s">
+      <c r="B186" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C185" t="s">
+      <c r="C186" t="s">
         <v>361</v>
       </c>
-      <c r="D185" s="1" t="s">
+      <c r="D186" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="E185" s="1" t="s">
+      <c r="E186" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G185">
+      <c r="G186">
         <v>1081235</v>
       </c>
-      <c r="I185" s="2" t="s">
+      <c r="I186" s="2" t="s">
         <v>581</v>
       </c>
-      <c r="K185" s="6" t="str">
+      <c r="K186" s="6" t="str">
         <f t="shared" si="8"/>
         <v>T = BC847C, 45 V, 100 mA, 250 mW, hfe=400</v>
       </c>
     </row>
-    <row r="186" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="A186" s="18" t="s">
+    <row r="187" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="A187" s="18" t="s">
         <v>364</v>
       </c>
-      <c r="B186" s="1" t="s">
+      <c r="B187" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C186" t="s">
+      <c r="C187" t="s">
         <v>363</v>
       </c>
-      <c r="D186" s="1" t="s">
+      <c r="D187" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="E186" s="1" t="s">
+      <c r="E187" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G186">
+      <c r="G187">
         <v>1081281</v>
       </c>
-      <c r="I186" s="2" t="s">
+      <c r="I187" s="2" t="s">
         <v>582</v>
       </c>
-      <c r="K186" s="6" t="str">
+      <c r="K187" s="6" t="str">
         <f t="shared" si="8"/>
         <v>T = BCX56, 80 V, 1 A, 500 mW, hfe=100</v>
       </c>
     </row>
-    <row r="187" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="A187" s="18" t="s">
+    <row r="188" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="A188" s="18" t="s">
         <v>373</v>
       </c>
-      <c r="B187" s="1" t="s">
+      <c r="B188" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C187" t="s">
+      <c r="C188" t="s">
         <v>372</v>
       </c>
-      <c r="D187" s="1" t="s">
+      <c r="D188" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="E187" s="1" t="s">
+      <c r="E188" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G187">
+      <c r="G188">
         <v>1829342</v>
       </c>
-      <c r="I187" s="2" t="s">
+      <c r="I188" s="2" t="s">
         <v>583</v>
       </c>
-      <c r="K187" s="6" t="str">
+      <c r="K188" s="6" t="str">
         <f t="shared" si="8"/>
         <v>T = PBSS4021NZ, 20 V, 8 A, 1.7 W, hfe=500</v>
       </c>
     </row>
-    <row r="188" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="C188"/>
-      <c r="G188"/>
-      <c r="K188" s="6" t="str">
+    <row r="189" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="C189"/>
+      <c r="G189"/>
+      <c r="K189" s="6" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
-    <row r="189" spans="1:11" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A189" s="7" t="s">
+    <row r="190" spans="1:11" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A190" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B189" s="7"/>
-      <c r="C189" s="7"/>
-      <c r="D189" s="7"/>
-      <c r="E189" s="7" t="s">
+      <c r="B190" s="7"/>
+      <c r="C190" s="7"/>
+      <c r="D190" s="7"/>
+      <c r="E190" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="K189" s="9" t="str">
+      <c r="K190" s="9" t="str">
         <f t="shared" si="8"/>
         <v>T = Transistor BJT PNP</v>
       </c>
     </row>
-    <row r="190" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="A190" s="18" t="s">
+    <row r="191" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="A191" s="18" t="s">
         <v>367</v>
       </c>
-      <c r="B190" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C190" t="s">
+      <c r="B191" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C191" t="s">
         <v>368</v>
       </c>
-      <c r="D190" s="1" t="s">
+      <c r="D191" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="E190" s="1" t="s">
+      <c r="E191" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G190">
+      <c r="G191">
         <v>1798070</v>
       </c>
-      <c r="I190" s="2" t="s">
+      <c r="I191" s="2" t="s">
         <v>586</v>
       </c>
-      <c r="K190" s="6" t="str">
+      <c r="K191" s="6" t="str">
         <f t="shared" si="8"/>
         <v>T = BC857C, -45 V, -100 mA, 250 mW, hfe=400</v>
       </c>
     </row>
-    <row r="191" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="A191" s="18" t="s">
+    <row r="192" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="A192" s="18" t="s">
         <v>369</v>
       </c>
-      <c r="B191" s="1" t="s">
+      <c r="B192" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C191" t="s">
+      <c r="C192" t="s">
         <v>370</v>
       </c>
-      <c r="D191" s="1" t="s">
+      <c r="D192" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="E191" s="1" t="s">
+      <c r="E192" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G191">
+      <c r="G192">
         <v>1081276</v>
       </c>
-      <c r="I191" s="2" t="s">
+      <c r="I192" s="2" t="s">
         <v>585</v>
       </c>
-      <c r="K191" s="6" t="str">
+      <c r="K192" s="6" t="str">
         <f t="shared" si="8"/>
         <v>T = BCX53, -80 V, -1 A, 500 mW, hfe=100</v>
       </c>
     </row>
-    <row r="192" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="A192" s="18" t="s">
+    <row r="193" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="A193" s="18" t="s">
         <v>623</v>
       </c>
-      <c r="B192" s="1" t="s">
+      <c r="B193" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C192" t="s">
+      <c r="C193" t="s">
         <v>371</v>
       </c>
-      <c r="D192" s="1" t="s">
+      <c r="D193" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="E192" s="1" t="s">
+      <c r="E193" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G192">
+      <c r="G193">
         <v>1829345</v>
       </c>
-      <c r="I192" s="33" t="s">
+      <c r="I193" s="33" t="s">
         <v>584</v>
       </c>
-      <c r="K192" s="6" t="str">
+      <c r="K193" s="6" t="str">
         <f t="shared" si="8"/>
         <v>T = PBSS4021, -20 V, -6.6 A, 1.7 W, hfe=350</v>
       </c>
     </row>
-    <row r="193" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="C193"/>
-      <c r="G193"/>
-      <c r="K193" s="6" t="str">
+    <row r="194" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="C194"/>
+      <c r="G194"/>
+      <c r="K194" s="6" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
-    <row r="194" spans="1:11" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A194" s="7" t="s">
+    <row r="195" spans="1:11" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A195" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B194" s="7"/>
-      <c r="C194" s="7"/>
-      <c r="D194" s="7"/>
-      <c r="E194" s="7" t="s">
+      <c r="B195" s="7"/>
+      <c r="C195" s="7"/>
+      <c r="D195" s="7"/>
+      <c r="E195" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="K194" s="9" t="str">
+      <c r="K195" s="9" t="str">
         <f t="shared" si="8"/>
         <v>T = Transistor MOSFET-N</v>
       </c>
     </row>
-    <row r="195" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="A195" s="18" t="s">
+    <row r="196" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="A196" s="18" t="s">
         <v>376</v>
       </c>
-      <c r="B195" s="1" t="s">
+      <c r="B196" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C195" t="s">
+      <c r="C196" t="s">
         <v>377</v>
       </c>
-      <c r="D195" s="1" t="s">
+      <c r="D196" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="E195" s="1" t="s">
+      <c r="E196" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G195">
+      <c r="G196">
         <v>2317616</v>
       </c>
-      <c r="I195" s="2" t="s">
+      <c r="I196" s="2" t="s">
         <v>587</v>
       </c>
-      <c r="K195" s="6" t="str">
+      <c r="K196" s="6" t="str">
         <f t="shared" si="8"/>
         <v>T = 2N7002, 60 V, 250 mA, 300 mW, Vgs=4.5 V, Rdson=1 Ω</v>
       </c>
     </row>
-    <row r="196" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="A196" s="18" t="s">
+    <row r="197" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="A197" s="18" t="s">
         <v>381</v>
       </c>
-      <c r="B196" s="1" t="s">
+      <c r="B197" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C196" t="s">
+      <c r="C197" t="s">
         <v>380</v>
       </c>
-      <c r="D196" s="1" t="s">
+      <c r="D197" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="E196" s="1" t="s">
+      <c r="E197" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G196">
+      <c r="G197">
         <v>2069567</v>
       </c>
-      <c r="I196" s="2" t="s">
+      <c r="I197" s="2" t="s">
         <v>588</v>
       </c>
-      <c r="K196" s="6" t="str">
+      <c r="K197" s="6" t="str">
         <f t="shared" si="8"/>
         <v>T = PMT21EN, 30 V, 7 A, 1.7 W, Vgs=1.5V, Rdson=20 mΩ</v>
       </c>
     </row>
-    <row r="197" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="A197" s="18" t="s">
+    <row r="198" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="A198" s="18" t="s">
         <v>416</v>
       </c>
-      <c r="B197" s="1" t="s">
+      <c r="B198" s="1" t="s">
         <v>384</v>
       </c>
-      <c r="C197" t="s">
+      <c r="C198" t="s">
         <v>415</v>
       </c>
-      <c r="D197" s="1" t="s">
+      <c r="D198" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="E197" s="1" t="s">
+      <c r="E198" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G197">
+      <c r="G198">
         <v>1013449</v>
       </c>
-      <c r="I197" s="2" t="s">
+      <c r="I198" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="K197" s="6" t="str">
+      <c r="K198" s="6" t="str">
         <f t="shared" si="8"/>
         <v>T = IRF7832PbF, 30 V, 20 A, 2.5 W, Vgs=2 V, Rdson=4 mΩ</v>
       </c>
     </row>
-    <row r="198" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="C198"/>
-      <c r="G198"/>
-      <c r="K198" s="6" t="str">
+    <row r="199" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="C199"/>
+      <c r="G199"/>
+      <c r="K199" s="6" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
-    <row r="199" spans="1:11" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A199" s="7" t="s">
+    <row r="200" spans="1:11" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A200" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B199" s="7"/>
-      <c r="C199" s="7"/>
-      <c r="D199" s="7"/>
-      <c r="E199" s="7" t="s">
+      <c r="B200" s="7"/>
+      <c r="C200" s="7"/>
+      <c r="D200" s="7"/>
+      <c r="E200" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="K199" s="9" t="str">
+      <c r="K200" s="9" t="str">
         <f t="shared" si="8"/>
         <v>T = Transistor MOSFET-P</v>
       </c>
     </row>
-    <row r="200" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="A200" s="18" t="s">
+    <row r="201" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="A201" s="18" t="s">
         <v>374</v>
       </c>
-      <c r="B200" s="1" t="s">
+      <c r="B201" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="C200" s="1" t="s">
+      <c r="C201" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="D200" s="1" t="s">
+      <c r="D201" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="E200" s="1" t="s">
+      <c r="E201" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G200" s="2">
+      <c r="G201" s="2">
         <v>1056526</v>
       </c>
-      <c r="I200" s="2" t="s">
+      <c r="I201" s="2" t="s">
         <v>589</v>
       </c>
-      <c r="K200" s="6" t="str">
+      <c r="K201" s="6" t="str">
         <f t="shared" si="8"/>
         <v>T = BSS84P, -60 V, -170 mA, 350 mW, Vgs=-1.5 V, Rdson=8 Ω</v>
       </c>
     </row>
-    <row r="201" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="A201" s="18" t="s">
+    <row r="202" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="A202" s="18" t="s">
         <v>382</v>
       </c>
-      <c r="B201" s="1" t="s">
+      <c r="B202" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="C201" s="1" t="s">
+      <c r="C202" s="1" t="s">
         <v>379</v>
       </c>
-      <c r="D201" s="1" t="s">
+      <c r="D202" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="E201" s="1" t="s">
+      <c r="E202" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G201" s="2">
+      <c r="G202" s="2">
         <v>7564945</v>
       </c>
-      <c r="I201" s="2" t="s">
+      <c r="I202" s="2" t="s">
         <v>590</v>
       </c>
-      <c r="K201" s="6" t="str">
+      <c r="K202" s="6" t="str">
         <f t="shared" si="8"/>
         <v>T = ZXMP4A16G, -40 V, -6 A, 2 W, Vgs=-2.5V, Rdson=0.1 Ω</v>
       </c>
     </row>
-    <row r="202" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="A202" s="18" t="s">
+    <row r="203" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="A203" s="18" t="s">
         <v>386</v>
       </c>
-      <c r="B202" s="1" t="s">
+      <c r="B203" s="1" t="s">
         <v>384</v>
       </c>
-      <c r="C202" s="1" t="s">
+      <c r="C203" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="D202" s="1" t="s">
+      <c r="D203" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="E202" s="1" t="s">
+      <c r="E203" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G202" s="2">
+      <c r="G203" s="2">
         <v>1831075</v>
       </c>
-      <c r="I202" s="2" t="s">
+      <c r="I203" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="K202" s="6" t="str">
+      <c r="K203" s="6" t="str">
         <f t="shared" si="8"/>
         <v>T = IRF9321PBF, -30 V, -15 A, 2.5 W, Vgs=-1.8 V, Rdson=30 mΩ</v>
       </c>
     </row>
-    <row r="203" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="K203" s="6" t="str">
+    <row r="204" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="K204" s="6" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
-    <row r="204" spans="1:11" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A204" s="7" t="s">
+    <row r="205" spans="1:11" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A205" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B204" s="14"/>
-      <c r="C204" s="14"/>
-      <c r="D204" s="14"/>
-      <c r="E204" s="14" t="s">
+      <c r="B205" s="14"/>
+      <c r="C205" s="14"/>
+      <c r="D205" s="14"/>
+      <c r="E205" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="K204" s="17"/>
-    </row>
-    <row r="205" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="A205" s="18" t="s">
-        <v>405</v>
-      </c>
-      <c r="B205" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C205" s="1" t="s">
-        <v>409</v>
-      </c>
-      <c r="D205" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="E205" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G205" s="34" t="s">
-        <v>408</v>
-      </c>
-      <c r="I205" s="2" t="s">
-        <v>410</v>
-      </c>
-      <c r="K205" s="6" t="str">
-        <f t="shared" ref="K205:K219" si="9">CONCATENATE(CONCATENATE($E205,IF(ISBLANK($E205),""," = "),$A205),IF(ISBLANK($J205),"",", "),$J205)</f>
-        <v>T = BF545A, N, 30 V, 6.5 mA, Vgs(off)=-2.2 V</v>
-      </c>
+      <c r="K205" s="17"/>
     </row>
     <row r="206" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A206" s="18" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B206" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C206" s="1" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="D206" s="1" t="s">
         <v>355</v>
@@ -7676,129 +7682,129 @@
       <c r="E206" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G206" s="2">
+      <c r="G206" s="34" t="s">
+        <v>408</v>
+      </c>
+      <c r="I206" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="K206" s="6" t="str">
+        <f t="shared" ref="K206:K220" si="9">CONCATENATE(CONCATENATE($E206,IF(ISBLANK($E206),""," = "),$A206),IF(ISBLANK($J206),"",", "),$J206)</f>
+        <v>T = BF545A, N, 30 V, 6.5 mA, Vgs(off)=-2.2 V</v>
+      </c>
+    </row>
+    <row r="207" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="A207" s="18" t="s">
+        <v>406</v>
+      </c>
+      <c r="B207" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C207" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="D207" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="E207" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G207" s="2">
         <v>1349656</v>
       </c>
-      <c r="I206" s="2" t="s">
+      <c r="I207" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="K206" s="6" t="str">
+      <c r="K207" s="6" t="str">
         <f t="shared" si="9"/>
         <v>T = BF545B, N, 30 V, 15 mA, Vgs(off)=-3.8 V</v>
       </c>
     </row>
-    <row r="207" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="A207" s="18" t="s">
+    <row r="208" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="A208" s="18" t="s">
         <v>407</v>
       </c>
-      <c r="B207" s="1" t="s">
+      <c r="B208" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C207" s="1" t="s">
+      <c r="C208" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="D207" s="1" t="s">
+      <c r="D208" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="E207" s="1" t="s">
+      <c r="E208" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G207" s="2">
+      <c r="G208" s="2">
         <v>1758055</v>
       </c>
-      <c r="I207" s="2" t="s">
+      <c r="I208" s="2" t="s">
         <v>411</v>
       </c>
-      <c r="K207" s="6" t="str">
+      <c r="K208" s="6" t="str">
         <f t="shared" si="9"/>
         <v>T = BF545C, N, 30 V, 25 mA, Vgs(off)=-7.8 V</v>
       </c>
     </row>
-    <row r="208" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="E208"/>
-      <c r="K208" s="6" t="str">
+    <row r="209" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="E209"/>
+      <c r="K209" s="6" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
-    <row r="209" spans="1:13" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A209" s="7" t="s">
+    <row r="210" spans="1:13" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A210" s="7" t="s">
         <v>388</v>
       </c>
-      <c r="B209" s="7"/>
-      <c r="C209" s="7"/>
-      <c r="D209" s="7"/>
-      <c r="E209" s="7" t="s">
+      <c r="B210" s="7"/>
+      <c r="C210" s="7"/>
+      <c r="D210" s="7"/>
+      <c r="E210" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="K209" s="9" t="str">
+      <c r="K210" s="9" t="str">
         <f t="shared" si="9"/>
         <v>X = Crystal &amp; oscillator</v>
       </c>
     </row>
-    <row r="210" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="A210" s="18" t="s">
+    <row r="211" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="A211" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="B210" s="1" t="s">
+      <c r="B211" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C210" s="1" t="s">
+      <c r="C211" s="1" t="s">
         <v>402</v>
       </c>
-      <c r="D210" s="18" t="s">
+      <c r="D211" s="18" t="s">
         <v>403</v>
       </c>
-      <c r="E210" s="1" t="s">
+      <c r="E211" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G210">
+      <c r="G211">
         <v>2308726</v>
       </c>
-      <c r="I210" s="2" t="s">
+      <c r="I211" s="2" t="s">
         <v>592</v>
       </c>
-      <c r="K210" s="6" t="str">
+      <c r="K211" s="6" t="str">
         <f t="shared" si="9"/>
         <v>X = 8 MHz, 18 pF</v>
       </c>
     </row>
-    <row r="211" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="A211" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="B211" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C211" s="2" t="s">
-        <v>401</v>
-      </c>
-      <c r="D211" s="18" t="s">
-        <v>403</v>
-      </c>
-      <c r="E211" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G211" s="2">
-        <v>1841963</v>
-      </c>
-      <c r="I211" s="2" t="s">
-        <v>594</v>
-      </c>
-      <c r="K211" s="6" t="str">
-        <f>CONCATENATE(CONCATENATE($E211,IF(ISBLANK($E211),""," = "),$A211),IF(ISBLANK($J211),"",", "),$J211)</f>
-        <v>X = 12 MHz, 18 pF</v>
-      </c>
-    </row>
     <row r="212" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A212" s="18" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B212" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C212" s="1" t="s">
-        <v>399</v>
+      <c r="C212" s="2" t="s">
+        <v>401</v>
       </c>
       <c r="D212" s="18" t="s">
         <v>403</v>
@@ -7807,25 +7813,25 @@
         <v>34</v>
       </c>
       <c r="G212" s="2">
-        <v>1841977</v>
+        <v>1841963</v>
       </c>
       <c r="I212" s="2" t="s">
-        <v>591</v>
+        <v>594</v>
       </c>
       <c r="K212" s="6" t="str">
         <f>CONCATENATE(CONCATENATE($E212,IF(ISBLANK($E212),""," = "),$A212),IF(ISBLANK($J212),"",", "),$J212)</f>
-        <v>X = 16 MHz, 18 pF</v>
+        <v>X = 12 MHz, 18 pF</v>
       </c>
     </row>
     <row r="213" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A213" s="18" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B213" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C213" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D213" s="18" t="s">
         <v>403</v>
@@ -7833,53 +7839,53 @@
       <c r="E213" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G213">
-        <v>1841988</v>
+      <c r="G213" s="2">
+        <v>1841977</v>
       </c>
       <c r="I213" s="2" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="K213" s="6" t="str">
         <f>CONCATENATE(CONCATENATE($E213,IF(ISBLANK($E213),""," = "),$A213),IF(ISBLANK($J213),"",", "),$J213)</f>
-        <v>X = 20 MHz, 18 pF</v>
+        <v>X = 16 MHz, 18 pF</v>
       </c>
     </row>
     <row r="214" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A214" s="18" t="s">
-        <v>397</v>
+        <v>45</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>391</v>
+        <v>47</v>
       </c>
       <c r="C214" s="1" t="s">
-        <v>398</v>
-      </c>
-      <c r="D214" s="1" t="s">
-        <v>404</v>
+        <v>400</v>
+      </c>
+      <c r="D214" s="18" t="s">
+        <v>403</v>
       </c>
       <c r="E214" s="1" t="s">
-        <v>389</v>
+        <v>34</v>
       </c>
       <c r="G214">
-        <v>2442991</v>
+        <v>1841988</v>
       </c>
       <c r="I214" s="2" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="K214" s="6" t="str">
         <f>CONCATENATE(CONCATENATE($E214,IF(ISBLANK($E214),""," = "),$A214),IF(ISBLANK($J214),"",", "),$J214)</f>
-        <v>OSC = 8 MHz, 15 pF, 3V3</v>
+        <v>X = 20 MHz, 18 pF</v>
       </c>
     </row>
     <row r="215" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A215" s="18" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="B215" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="C215" t="s">
-        <v>390</v>
+      <c r="C215" s="1" t="s">
+        <v>398</v>
       </c>
       <c r="D215" s="1" t="s">
         <v>404</v>
@@ -7887,26 +7893,26 @@
       <c r="E215" s="1" t="s">
         <v>389</v>
       </c>
-      <c r="G215" s="2">
-        <v>2442993</v>
+      <c r="G215">
+        <v>2442991</v>
       </c>
       <c r="I215" s="2" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="K215" s="6" t="str">
         <f>CONCATENATE(CONCATENATE($E215,IF(ISBLANK($E215),""," = "),$A215),IF(ISBLANK($J215),"",", "),$J215)</f>
-        <v>OSC = 12 MHz, 15 pF, 3V3</v>
+        <v>OSC = 8 MHz, 15 pF, 3V3</v>
       </c>
     </row>
     <row r="216" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A216" s="18" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B216" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="C216" s="1" t="s">
-        <v>392</v>
+      <c r="C216" t="s">
+        <v>390</v>
       </c>
       <c r="D216" s="1" t="s">
         <v>404</v>
@@ -7914,477 +7920,498 @@
       <c r="E216" s="1" t="s">
         <v>389</v>
       </c>
-      <c r="G216">
+      <c r="G216" s="2">
+        <v>2442993</v>
+      </c>
+      <c r="I216" s="2" t="s">
+        <v>597</v>
+      </c>
+      <c r="K216" s="6" t="str">
+        <f>CONCATENATE(CONCATENATE($E216,IF(ISBLANK($E216),""," = "),$A216),IF(ISBLANK($J216),"",", "),$J216)</f>
+        <v>OSC = 12 MHz, 15 pF, 3V3</v>
+      </c>
+    </row>
+    <row r="217" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="A217" s="18" t="s">
+        <v>395</v>
+      </c>
+      <c r="B217" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="C217" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="D217" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="E217" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="G217">
         <v>2442979</v>
       </c>
-      <c r="I216" s="2" t="s">
+      <c r="I217" s="2" t="s">
         <v>598</v>
       </c>
-      <c r="K216" s="6" t="str">
+      <c r="K217" s="6" t="str">
         <f t="shared" si="9"/>
         <v>OSC = 16 MHz, 15 pF, 3V3</v>
       </c>
     </row>
-    <row r="217" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="A217" s="18" t="s">
+    <row r="218" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="A218" s="18" t="s">
         <v>396</v>
       </c>
-      <c r="B217" s="1" t="s">
+      <c r="B218" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="C217" s="1" t="s">
+      <c r="C218" s="1" t="s">
         <v>393</v>
       </c>
-      <c r="D217" s="1" t="s">
+      <c r="D218" s="1" t="s">
         <v>404</v>
       </c>
-      <c r="E217" s="1" t="s">
+      <c r="E218" s="1" t="s">
         <v>389</v>
       </c>
-      <c r="G217">
+      <c r="G218">
         <v>2442997</v>
       </c>
-      <c r="I217" s="2" t="s">
+      <c r="I218" s="2" t="s">
         <v>596</v>
       </c>
-      <c r="K217" s="6" t="str">
+      <c r="K218" s="6" t="str">
         <f t="shared" si="9"/>
         <v>OSC = 20 MHz, 15 pF, 3V3</v>
       </c>
     </row>
-    <row r="218" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="G218"/>
-      <c r="K218" s="6" t="str">
+    <row r="219" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="G219"/>
+      <c r="K219" s="6" t="str">
         <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
-    <row r="219" spans="1:13" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A219" s="7" t="s">
+    <row r="220" spans="1:13" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A220" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B219" s="7"/>
-      <c r="C219" s="7"/>
-      <c r="D219" s="7"/>
-      <c r="E219" s="7" t="s">
+      <c r="B220" s="7"/>
+      <c r="C220" s="7"/>
+      <c r="D220" s="7"/>
+      <c r="E220" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="K219" s="9" t="str">
+      <c r="K220" s="9" t="str">
         <f t="shared" si="9"/>
         <v>K = Connector &amp; socket</v>
       </c>
     </row>
-    <row r="220" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="A220" s="18" t="s">
+    <row r="221" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="A221" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="B220" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C220" s="1" t="s">
+      <c r="B221" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C221" s="1" t="s">
         <v>421</v>
       </c>
-      <c r="D220" s="32" t="s">
+      <c r="D221" s="32" t="s">
         <v>423</v>
       </c>
-      <c r="E220" s="5" t="s">
+      <c r="E221" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="G220" s="2">
+      <c r="G221" s="2">
         <v>1696546</v>
       </c>
-      <c r="I220" s="19" t="s">
+      <c r="I221" s="19" t="s">
         <v>603</v>
       </c>
-      <c r="K220" s="6" t="str">
-        <f t="shared" ref="K220:K225" si="10">CONCATENATE(CONCATENATE($E220,IF(ISBLANK($E220),""," = "),$A220),IF(ISBLANK($J220),"",", "),$J220)</f>
+      <c r="K221" s="6" t="str">
+        <f t="shared" ref="K221:K226" si="10">CONCATENATE(CONCATENATE($E221,IF(ISBLANK($E221),""," = "),$A221),IF(ISBLANK($J221),"",", "),$J221)</f>
         <v>K = USB type A plug, right angle</v>
       </c>
-    </row>
-    <row r="221" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A221" s="25" t="s">
-        <v>419</v>
-      </c>
-      <c r="B221" s="25" t="s">
-        <v>418</v>
-      </c>
-      <c r="C221" s="25" t="s">
-        <v>420</v>
-      </c>
-      <c r="D221" s="25" t="s">
-        <v>422</v>
-      </c>
-      <c r="E221" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="F221" s="27"/>
-      <c r="G221" s="28">
-        <v>1125348</v>
-      </c>
-      <c r="H221" s="27"/>
-      <c r="I221" s="29" t="s">
-        <v>599</v>
-      </c>
-      <c r="J221" s="27"/>
-      <c r="K221" s="30" t="str">
-        <f t="shared" si="10"/>
-        <v>K = Mini USB type B receptacle</v>
-      </c>
-      <c r="L221" s="27"/>
-      <c r="M221" s="27"/>
     </row>
     <row r="222" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A222" s="25" t="s">
-        <v>616</v>
+        <v>419</v>
       </c>
       <c r="B222" s="25" t="s">
         <v>418</v>
       </c>
       <c r="C222" s="25" t="s">
-        <v>614</v>
+        <v>420</v>
       </c>
       <c r="D222" s="25" t="s">
-        <v>615</v>
-      </c>
-      <c r="E222" s="25" t="s">
+        <v>422</v>
+      </c>
+      <c r="E222" s="26" t="s">
         <v>35</v>
       </c>
       <c r="F222" s="27"/>
-      <c r="G222" s="31">
-        <v>1568026</v>
+      <c r="G222" s="28">
+        <v>1125348</v>
       </c>
       <c r="H222" s="27"/>
       <c r="I222" s="29" t="s">
-        <v>631</v>
+        <v>599</v>
       </c>
       <c r="J222" s="27"/>
       <c r="K222" s="30" t="str">
         <f t="shared" si="10"/>
-        <v>K = Micro USB type B receptacle, bottom mount</v>
+        <v>K = Mini USB type B receptacle</v>
       </c>
       <c r="L222" s="27"/>
       <c r="M222" s="27"/>
     </row>
-    <row r="224" spans="1:13" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A224" s="14" t="s">
+    <row r="223" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A223" s="25" t="s">
+        <v>616</v>
+      </c>
+      <c r="B223" s="25" t="s">
+        <v>418</v>
+      </c>
+      <c r="C223" s="25" t="s">
+        <v>614</v>
+      </c>
+      <c r="D223" s="25" t="s">
+        <v>615</v>
+      </c>
+      <c r="E223" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="F223" s="27"/>
+      <c r="G223" s="31">
+        <v>1568026</v>
+      </c>
+      <c r="H223" s="27"/>
+      <c r="I223" s="29" t="s">
+        <v>631</v>
+      </c>
+      <c r="J223" s="27"/>
+      <c r="K223" s="30" t="str">
+        <f t="shared" si="10"/>
+        <v>K = Micro USB type B receptacle, bottom mount</v>
+      </c>
+      <c r="L223" s="27"/>
+      <c r="M223" s="27"/>
+    </row>
+    <row r="225" spans="1:11" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A225" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="B224" s="12"/>
-      <c r="C224" s="12"/>
-      <c r="D224" s="12"/>
-      <c r="E224" s="14"/>
-      <c r="K224" s="9" t="str">
+      <c r="B225" s="12"/>
+      <c r="C225" s="12"/>
+      <c r="D225" s="12"/>
+      <c r="E225" s="14"/>
+      <c r="K225" s="9" t="str">
         <f t="shared" si="10"/>
         <v>Switch &amp; relay</v>
       </c>
     </row>
-    <row r="225" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A225" s="18" t="s">
+    <row r="226" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A226" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="B225" s="1" t="s">
+      <c r="B226" s="1" t="s">
         <v>424</v>
       </c>
-      <c r="C225" s="1" t="s">
+      <c r="C226" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="D225" s="1" t="s">
+      <c r="D226" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="E225" s="1" t="s">
+      <c r="E226" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G225" s="2">
+      <c r="G226" s="2">
         <v>2320038</v>
       </c>
-      <c r="I225" s="2" t="s">
+      <c r="I226" s="2" t="s">
         <v>604</v>
       </c>
-      <c r="K225" s="30" t="str">
+      <c r="K226" s="30" t="str">
         <f t="shared" si="10"/>
         <v>S = Switch, tactile, 24 V, 50 mA, 6x6 mm</v>
       </c>
     </row>
-    <row r="226" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="K226" s="6"/>
-    </row>
-    <row r="227" spans="1:11" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A227" s="7" t="s">
+    <row r="227" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="K227" s="6"/>
+    </row>
+    <row r="228" spans="1:11" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A228" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="B227" s="7"/>
-      <c r="C227" s="7"/>
-      <c r="D227" s="7"/>
-      <c r="E227" s="7" t="s">
+      <c r="B228" s="7"/>
+      <c r="C228" s="7"/>
+      <c r="D228" s="7"/>
+      <c r="E228" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="K227" s="9" t="str">
-        <f t="shared" ref="K227:K235" si="11">CONCATENATE(CONCATENATE($E227,IF(ISBLANK($E227),""," = "),$A227),IF(ISBLANK($J227),"",", "),$J227)</f>
+      <c r="K228" s="9" t="str">
+        <f t="shared" ref="K228:K236" si="11">CONCATENATE(CONCATENATE($E228,IF(ISBLANK($E228),""," = "),$A228),IF(ISBLANK($J228),"",", "),$J228)</f>
         <v>IC = Voltage regulator</v>
       </c>
     </row>
-    <row r="228" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A228" s="18" t="s">
+    <row r="229" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A229" s="18" t="s">
         <v>437</v>
       </c>
-      <c r="B228" s="1" t="s">
+      <c r="B229" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C228" s="1" t="s">
+      <c r="C229" s="1" t="s">
         <v>433</v>
       </c>
-      <c r="D228" s="1" t="s">
+      <c r="D229" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="E228" s="1" t="s">
+      <c r="E229" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G228" s="2">
+      <c r="G229" s="2">
         <v>1296592</v>
       </c>
-      <c r="I228" s="2" t="s">
+      <c r="I229" s="2" t="s">
         <v>434</v>
       </c>
-      <c r="K228" s="30" t="str">
+      <c r="K229" s="30" t="str">
         <f t="shared" si="11"/>
         <v>IC = MCP1700, LDO, 3.3 V, 0.1 A</v>
       </c>
     </row>
-    <row r="229" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A229" s="18" t="s">
+    <row r="230" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A230" s="18" t="s">
         <v>428</v>
       </c>
-      <c r="B229" s="1" t="s">
+      <c r="B230" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C229" s="2" t="s">
+      <c r="C230" s="2" t="s">
         <v>426</v>
       </c>
-      <c r="D229" s="1" t="s">
+      <c r="D230" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="E229" s="1" t="s">
+      <c r="E230" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G229" s="2">
+      <c r="G230" s="2">
         <v>9755314</v>
       </c>
-      <c r="I229" s="2" t="s">
+      <c r="I230" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="K229" s="30" t="str">
+      <c r="K230" s="30" t="str">
         <f t="shared" si="11"/>
         <v>IC = KF33, LDO, 3.3 V, 0.5 A</v>
       </c>
     </row>
-    <row r="230" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A230" s="18" t="s">
+    <row r="231" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A231" s="18" t="s">
         <v>442</v>
       </c>
-      <c r="B230" s="1" t="s">
+      <c r="B231" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C230" s="1" t="s">
+      <c r="C231" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="D230" s="1" t="s">
+      <c r="D231" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="E230" s="1" t="s">
+      <c r="E231" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G230" s="2">
+      <c r="G231" s="2">
         <v>1087169</v>
       </c>
-      <c r="I230" s="2" t="s">
+      <c r="I231" s="2" t="s">
         <v>439</v>
       </c>
-      <c r="K230" s="30" t="str">
+      <c r="K231" s="30" t="str">
         <f t="shared" si="11"/>
         <v>IC = LD1117DT33, LDO, 3.3 V, 0.8 A</v>
       </c>
     </row>
-    <row r="231" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A231" s="18" t="s">
+    <row r="232" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A232" s="18" t="s">
         <v>438</v>
       </c>
-      <c r="B231" s="1" t="s">
+      <c r="B232" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C231" s="1" t="s">
+      <c r="C232" s="1" t="s">
         <v>436</v>
       </c>
-      <c r="D231" s="1" t="s">
+      <c r="D232" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="E231" s="1" t="s">
+      <c r="E232" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G231" s="2">
+      <c r="G232" s="2">
         <v>1296593</v>
       </c>
-      <c r="I231" s="2" t="s">
+      <c r="I232" s="2" t="s">
         <v>435</v>
       </c>
-      <c r="K231" s="30" t="str">
+      <c r="K232" s="30" t="str">
         <f t="shared" si="11"/>
         <v>IC = MCP1700, LDO, 5.0 V, 0.1 A</v>
       </c>
     </row>
-    <row r="232" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A232" s="18" t="s">
+    <row r="233" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A233" s="18" t="s">
         <v>430</v>
       </c>
-      <c r="B232" s="1" t="s">
+      <c r="B233" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C232" s="2" t="s">
+      <c r="C233" s="2" t="s">
         <v>429</v>
       </c>
-      <c r="D232" s="1" t="s">
+      <c r="D233" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="E232" s="1" t="s">
+      <c r="E233" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G232" s="2">
+      <c r="G233" s="2">
         <v>9755373</v>
       </c>
-      <c r="I232" s="2" t="s">
+      <c r="I233" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="K232" s="30" t="str">
+      <c r="K233" s="30" t="str">
         <f t="shared" si="11"/>
         <v>IC = KF50, LDO, 5 V, 0.5 A</v>
       </c>
     </row>
-    <row r="233" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A233" s="18" t="s">
+    <row r="234" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A234" s="18" t="s">
         <v>441</v>
       </c>
-      <c r="B233" s="1" t="s">
+      <c r="B234" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C233" s="2" t="s">
+      <c r="C234" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="D233" s="1" t="s">
+      <c r="D234" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="E233" s="1" t="s">
+      <c r="E234" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G233" s="2">
+      <c r="G234" s="2">
         <v>1703369</v>
       </c>
-      <c r="I233" s="2" t="s">
+      <c r="I234" s="2" t="s">
         <v>443</v>
       </c>
-      <c r="K233" s="30" t="str">
+      <c r="K234" s="30" t="str">
         <f t="shared" si="11"/>
         <v>IC = NCP5501, LDO, 5 V, 0.5 A</v>
       </c>
     </row>
-    <row r="234" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A234" s="18" t="s">
+    <row r="235" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A235" s="18" t="s">
         <v>628</v>
       </c>
-      <c r="B234" s="18" t="s">
+      <c r="B235" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="C234" s="19" t="s">
+      <c r="C235" s="19" t="s">
         <v>626</v>
       </c>
-      <c r="D234" s="18" t="s">
+      <c r="D235" s="18" t="s">
         <v>383</v>
       </c>
-      <c r="E234" s="18" t="s">
+      <c r="E235" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="F234" s="19"/>
-      <c r="G234" s="19">
+      <c r="F235" s="19"/>
+      <c r="G235" s="19">
         <v>1053582</v>
       </c>
-      <c r="H234" s="19"/>
-      <c r="I234" s="19" t="s">
+      <c r="H235" s="19"/>
+      <c r="I235" s="19" t="s">
         <v>629</v>
       </c>
-      <c r="K234" s="30" t="str">
+      <c r="K235" s="30" t="str">
         <f t="shared" si="11"/>
         <v>IC = MC34063A Boost/buck/inverting regulator, 1.5 A</v>
       </c>
     </row>
-    <row r="235" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A235" s="18" t="s">
+    <row r="236" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A236" s="18" t="s">
         <v>627</v>
       </c>
-      <c r="B235" s="18" t="s">
+      <c r="B236" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="C235" s="18" t="s">
+      <c r="C236" s="18" t="s">
         <v>625</v>
       </c>
-      <c r="D235" s="18" t="s">
+      <c r="D236" s="18" t="s">
         <v>639</v>
       </c>
-      <c r="E235" s="18" t="s">
+      <c r="E236" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="F235" s="19"/>
-      <c r="G235" s="19">
+      <c r="F236" s="19"/>
+      <c r="G236" s="19">
         <v>1685537</v>
       </c>
-      <c r="H235" s="19"/>
-      <c r="I235" s="19" t="s">
+      <c r="H236" s="19"/>
+      <c r="I236" s="19" t="s">
         <v>630</v>
       </c>
-      <c r="K235" s="30" t="str">
+      <c r="K236" s="30" t="str">
         <f t="shared" si="11"/>
         <v>IC = LM2576-ADJ, Step-down regulator, 1.5 - 37 V, 3 A</v>
       </c>
     </row>
-    <row r="237" spans="1:11" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A237" s="7" t="s">
+    <row r="238" spans="1:11" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A238" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="B237" s="7"/>
-      <c r="C237" s="7"/>
-      <c r="D237" s="7"/>
-      <c r="E237" s="7"/>
-      <c r="K237" s="9" t="str">
-        <f t="shared" ref="K237" si="12">CONCATENATE(CONCATENATE($E237,IF(ISBLANK($E237),""," = "),$A237),IF(ISBLANK($J237),"",", "),$J237)</f>
+      <c r="B238" s="7"/>
+      <c r="C238" s="7"/>
+      <c r="D238" s="7"/>
+      <c r="E238" s="7"/>
+      <c r="K238" s="9" t="str">
+        <f t="shared" ref="K238" si="12">CONCATENATE(CONCATENATE($E238,IF(ISBLANK($E238),""," = "),$A238),IF(ISBLANK($J238),"",", "),$J238)</f>
         <v>Miscelaneous</v>
       </c>
     </row>
-    <row r="240" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A240" s="21" t="s">
+    <row r="241" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A241" s="21" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="242" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A242" s="22" t="s">
+    <row r="243" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A243" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="B242" s="23"/>
-      <c r="C242" s="23"/>
-    </row>
-    <row r="243" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A243" s="1" t="s">
+      <c r="B243" s="23"/>
+      <c r="C243" s="23"/>
+    </row>
+    <row r="244" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A244" s="1" t="s">
         <v>640</v>
       </c>
-      <c r="C243" s="1" t="s">
+      <c r="C244" s="1" t="s">
         <v>641</v>
       </c>
     </row>
-    <row r="246" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="K246" s="6" t="str">
-        <f>CONCATENATE(CONCATENATE($E246,IF(ISBLANK($E246),""," = "),$A246),IF(ISBLANK($J246),"",", "),$J246)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="248" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="K248" s="6" t="str">
-        <f>CONCATENATE(CONCATENATE($E248,IF(ISBLANK($E248),""," = "),$A248),IF(ISBLANK($J248),"",", "),$J248)</f>
+    <row r="247" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="K247" s="6" t="str">
+        <f>CONCATENATE(CONCATENATE($E247,IF(ISBLANK($E247),""," = "),$A247),IF(ISBLANK($J247),"",", "),$J247)</f>
         <v/>
       </c>
     </row>
@@ -8394,12 +8421,11 @@
         <v/>
       </c>
     </row>
-    <row r="250" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A250" s="2"/>
-      <c r="B250" s="2"/>
-      <c r="C250" s="2"/>
-      <c r="D250" s="2"/>
-      <c r="E250" s="2"/>
+    <row r="250" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="K250" s="6" t="str">
+        <f>CONCATENATE(CONCATENATE($E250,IF(ISBLANK($E250),""," = "),$A250),IF(ISBLANK($J250),"",", "),$J250)</f>
+        <v/>
+      </c>
     </row>
     <row r="251" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A251" s="2"/>
@@ -8408,15 +8434,16 @@
       <c r="D251" s="2"/>
       <c r="E251" s="2"/>
     </row>
-    <row r="252" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="K252" s="6" t="str">
-        <f t="shared" ref="K252:K283" si="13">CONCATENATE(CONCATENATE($E252,IF(ISBLANK($E252),""," = "),$A252),IF(ISBLANK($J252),"",", "),$J252)</f>
-        <v/>
-      </c>
+    <row r="252" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A252" s="2"/>
+      <c r="B252" s="2"/>
+      <c r="C252" s="2"/>
+      <c r="D252" s="2"/>
+      <c r="E252" s="2"/>
     </row>
     <row r="253" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="K253" s="6" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="K253:K284" si="13">CONCATENATE(CONCATENATE($E253,IF(ISBLANK($E253),""," = "),$A253),IF(ISBLANK($J253),"",", "),$J253)</f>
         <v/>
       </c>
     </row>
@@ -8602,13 +8629,13 @@
     </row>
     <row r="284" spans="11:11" ht="15" x14ac:dyDescent="0.2">
       <c r="K284" s="6" t="str">
-        <f t="shared" ref="K284:K302" si="14">CONCATENATE(CONCATENATE($E284,IF(ISBLANK($E284),""," = "),$A284),IF(ISBLANK($J284),"",", "),$J284)</f>
+        <f t="shared" si="13"/>
         <v/>
       </c>
     </row>
     <row r="285" spans="11:11" ht="15" x14ac:dyDescent="0.2">
       <c r="K285" s="6" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" ref="K285:K303" si="14">CONCATENATE(CONCATENATE($E285,IF(ISBLANK($E285),""," = "),$A285),IF(ISBLANK($J285),"",", "),$J285)</f>
         <v/>
       </c>
     </row>
@@ -8710,6 +8737,12 @@
     </row>
     <row r="302" spans="11:11" ht="15" x14ac:dyDescent="0.2">
       <c r="K302" s="6" t="str">
+        <f t="shared" si="14"/>
+        <v/>
+      </c>
+    </row>
+    <row r="303" spans="11:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="K303" s="6" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>

</xml_diff>